<commit_message>
R 0.1.4 (Trends, Stream OpenAI)
</commit_message>
<xml_diff>
--- a/data/openai-examples-21.xlsx
+++ b/data/openai-examples-21.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/msehgal/Developer/amazon-bedrock-workshop/ai4e_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manavsehgal/Developer/gtsystem/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{C39432E4-B533-F847-A920-BE8FEE02D12F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0984B033-0225-AA4F-807C-20AEFA143B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{9F43A9F2-79FE-1449-91C1-BB5BE0D54040}"/>
+    <workbookView xWindow="380" yWindow="760" windowWidth="28040" windowHeight="16940" xr2:uid="{9F43A9F2-79FE-1449-91C1-BB5BE0D54040}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="60">
   <si>
     <t>Task</t>
   </si>
@@ -43,12 +43,6 @@
     <t>Grammar correction</t>
   </si>
   <si>
-    <t>Task Types</t>
-  </si>
-  <si>
-    <t>Transform; Natural Language</t>
-  </si>
-  <si>
     <t>System</t>
   </si>
   <si>
@@ -61,24 +55,9 @@
     <t>She no went to the market.</t>
   </si>
   <si>
-    <t>Source</t>
-  </si>
-  <si>
-    <t>OpenAI Examples</t>
-  </si>
-  <si>
-    <t>Temperature</t>
-  </si>
-  <si>
-    <t>TopP</t>
-  </si>
-  <si>
     <t>Summarize for a 2nd grader</t>
   </si>
   <si>
-    <t>Extract; Natural Language</t>
-  </si>
-  <si>
     <t>Summarize content you are provided with for a second-grade student.</t>
   </si>
   <si>
@@ -104,9 +83,6 @@
   </si>
   <si>
     <t>Calculate time complexity</t>
-  </si>
-  <si>
-    <t>Transform; Code</t>
   </si>
   <si>
     <t>You will be provided with Python code, and your task is to calculate its time complexity.</t>
@@ -124,9 +100,6 @@
   </si>
   <si>
     <t>You will be provided with a piece of code, and your task is to explain it in a concise way.</t>
-  </si>
-  <si>
-    <t>Extract; Code</t>
   </si>
   <si>
     <t>class Log:
@@ -169,9 +142,6 @@
     <t>Product name generator</t>
   </si>
   <si>
-    <t>Generate; Natural Language</t>
-  </si>
-  <si>
     <t>You will be provided with a product description and seed words, and your task is to generate product names.</t>
   </si>
   <si>
@@ -200,9 +170,6 @@
     <t>Spreadsheet creator</t>
   </si>
   <si>
-    <t>Generate; Structured Data</t>
-  </si>
-  <si>
     <t>Create a two-column CSV of top science fiction movies along with the year of release.</t>
   </si>
   <si>
@@ -230,9 +197,6 @@
     <t>Mood to color</t>
   </si>
   <si>
-    <t>Extract; Structured Data</t>
-  </si>
-  <si>
     <t>You will be provided with a description of a mood, and your task is to generate the CSS code for a color that matches it. Write your output in json with a single key called "css_code".</t>
   </si>
   <si>
@@ -261,9 +225,6 @@
   </si>
   <si>
     <t>Function from specification</t>
-  </si>
-  <si>
-    <t>Generate; Code</t>
   </si>
   <si>
     <t>Write a Python function that takes as input a file path to an image, loads the image into memory as a numpy array, then crops the rows and columns around the perimeter if they are darker than a threshold value. Use the mean value of rows and columns to decide if they should be marked for deletion.</t>
@@ -382,9 +343,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -422,7 +383,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -528,7 +489,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -670,7 +631,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -678,28 +639,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5239C200-DC00-F547-9D96-B86C4B0BB380}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="165" zoomScaleNormal="165" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C18" sqref="C18"/>
+      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="60.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="55.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="60.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="55.6640625" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -707,502 +664,238 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="170" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="1">
-        <v>0.7</v>
-      </c>
-      <c r="F2" s="1">
-        <v>1</v>
-      </c>
-      <c r="G2" s="1" t="s">
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="153" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="170" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="1" t="s">
+    </row>
+    <row r="6" spans="1:3" ht="102" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="1">
-        <v>0.7</v>
-      </c>
-      <c r="F3" s="1">
-        <v>1</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="153" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="1" t="s">
+    </row>
+    <row r="7" spans="1:3" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="1">
-        <v>0.7</v>
-      </c>
-      <c r="F4" s="1">
-        <v>1</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="1" t="s">
+    </row>
+    <row r="8" spans="1:3" ht="238" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="F5" s="1">
-        <v>1</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="102" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="1" t="s">
+    </row>
+    <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="1">
-        <v>0.7</v>
-      </c>
-      <c r="F6" s="1">
-        <v>1</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="1" t="s">
+    </row>
+    <row r="10" spans="1:3" ht="170" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="1">
-        <v>0.7</v>
-      </c>
-      <c r="F7" s="1">
-        <v>1</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="238" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+    </row>
+    <row r="11" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="1" t="s">
+      <c r="B11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="1" t="s">
+    </row>
+    <row r="12" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="E8" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="F8" s="1">
-        <v>1</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E9" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="F9" s="1">
-        <v>1</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="170" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E10" s="1">
-        <v>0.7</v>
-      </c>
-      <c r="F10" s="1">
-        <v>1</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E11" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="F11" s="1">
-        <v>1</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E12" s="1">
-        <v>0.7</v>
-      </c>
-      <c r="F12" s="1">
-        <v>1</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E13" s="1">
-        <v>0.7</v>
-      </c>
-      <c r="F13" s="1">
-        <v>1</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E14" s="1">
-        <v>0.7</v>
-      </c>
-      <c r="F14" s="1">
-        <v>1</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D15" s="1" t="s">
+    </row>
+    <row r="16" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="85" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="255" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E15" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="F15" s="1">
-        <v>1</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
+    </row>
+    <row r="21" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" s="1" t="s">
+      <c r="B21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D16" s="1" t="s">
+    </row>
+    <row r="22" spans="1:3" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E16" s="1">
-        <v>0.3</v>
-      </c>
-      <c r="F16" s="1">
-        <v>1</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
+      <c r="B22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E17" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="F17" s="1">
-        <v>1</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="85" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E18" s="1">
-        <v>0.7</v>
-      </c>
-      <c r="F18" s="1">
-        <v>1</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="255" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E19" s="1">
-        <v>0.7</v>
-      </c>
-      <c r="F19" s="1">
-        <v>1</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="68" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E20" s="1">
-        <v>0.7</v>
-      </c>
-      <c r="F20" s="1">
-        <v>1</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E21" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="F21" s="1">
-        <v>1</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E22" s="1">
-        <v>0.7</v>
-      </c>
-      <c r="F22" s="1">
-        <v>1</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>